<commit_message>
Update result and slide
</commit_message>
<xml_diff>
--- a/results/lethal_accidents/lethal_accidents.xlsx
+++ b/results/lethal_accidents/lethal_accidents.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -527,9 +527,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Colore 1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1446,7 +1447,7 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1</c:v>
@@ -1464,7 +1465,7 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>1</c:v>
@@ -1509,7 +1510,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>8</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>6</c:v>
@@ -1518,7 +1519,7 @@
                   <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>11</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>3</c:v>
@@ -1542,7 +1543,7 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>10</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>5</c:v>
@@ -1557,7 +1558,7 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="40">
                   <c:v>1</c:v>
@@ -1593,7 +1594,7 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>6</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="52">
                   <c:v>6</c:v>
@@ -1611,13 +1612,13 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>8</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="58">
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>9</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="60">
                   <c:v>5</c:v>
@@ -1626,7 +1627,7 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>8</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="63">
                   <c:v>5</c:v>
@@ -1650,16 +1651,16 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>8</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>8</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="72">
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>12</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="74">
                   <c:v>5</c:v>
@@ -1668,7 +1669,7 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>8</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="77">
                   <c:v>5</c:v>
@@ -1695,7 +1696,7 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="86">
                   <c:v>1</c:v>
@@ -1713,7 +1714,7 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>9</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="92">
                   <c:v>3</c:v>
@@ -1734,7 +1735,7 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>10</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="99">
                   <c:v>3</c:v>
@@ -1764,7 +1765,7 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>8</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="109">
                   <c:v>2</c:v>
@@ -1782,10 +1783,10 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="114">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="115">
                   <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="115">
-                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="116">
                   <c:v>8</c:v>
@@ -1797,7 +1798,7 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="120">
                   <c:v>5</c:v>
@@ -1806,7 +1807,7 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>10</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="123">
                   <c:v>5</c:v>
@@ -1863,13 +1864,13 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="141">
-                  <c:v>7</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="142">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="143">
-                  <c:v>8</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="144">
                   <c:v>2</c:v>
@@ -1881,7 +1882,7 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="147">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="148">
                   <c:v>6</c:v>
@@ -1908,7 +1909,7 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="156">
-                  <c:v>8</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="157">
                   <c:v>5</c:v>
@@ -1950,7 +1951,7 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="170">
-                  <c:v>6</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="171">
                   <c:v>9</c:v>
@@ -1971,7 +1972,7 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="177">
-                  <c:v>6</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="178">
                   <c:v>10</c:v>
@@ -2004,7 +2005,7 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="188">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="189">
                   <c:v>6</c:v>
@@ -2034,7 +2035,7 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="198">
-                  <c:v>6</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="199">
                   <c:v>6</c:v>
@@ -2052,7 +2053,7 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="204">
-                  <c:v>13</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="205">
                   <c:v>3</c:v>
@@ -2073,7 +2074,7 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="211">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="212">
                   <c:v>6</c:v>
@@ -2085,7 +2086,7 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="215">
-                  <c:v>10</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="216">
                   <c:v>3</c:v>
@@ -2136,7 +2137,7 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="232">
-                  <c:v>7</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="233">
                   <c:v>1</c:v>
@@ -4852,7 +4853,7 @@
   <dimension ref="A1:F237"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4900,7 +4901,7 @@
         <f>(B2-2012)*52+C2-25</f>
         <v>1</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="2">
         <v>1</v>
       </c>
     </row>
@@ -4922,7 +4923,7 @@
         <f t="shared" ref="E3:E66" si="1">(B3-2012)*52+C3-25</f>
         <v>2</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="2">
         <v>4</v>
       </c>
     </row>
@@ -4944,7 +4945,7 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="2">
         <v>5</v>
       </c>
     </row>
@@ -4966,8 +4967,8 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="F5">
-        <v>10</v>
+      <c r="F5" s="2">
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -4988,7 +4989,7 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="2">
         <v>1</v>
       </c>
     </row>
@@ -5010,7 +5011,7 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="2">
         <v>5</v>
       </c>
     </row>
@@ -5032,7 +5033,7 @@
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="2">
         <v>7</v>
       </c>
     </row>
@@ -5054,7 +5055,7 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="2">
         <v>1</v>
       </c>
     </row>
@@ -5076,7 +5077,7 @@
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="2">
         <v>10</v>
       </c>
     </row>
@@ -5098,8 +5099,8 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="F11">
-        <v>7</v>
+      <c r="F11" s="2">
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -5120,7 +5121,7 @@
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="2">
         <v>1</v>
       </c>
     </row>
@@ -5142,7 +5143,7 @@
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="2">
         <v>7</v>
       </c>
     </row>
@@ -5164,7 +5165,7 @@
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="2">
         <v>8</v>
       </c>
     </row>
@@ -5186,7 +5187,7 @@
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="2">
         <v>9</v>
       </c>
     </row>
@@ -5208,7 +5209,7 @@
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="2">
         <v>2</v>
       </c>
     </row>
@@ -5230,7 +5231,7 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="2">
         <v>3</v>
       </c>
     </row>
@@ -5252,7 +5253,7 @@
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="2">
         <v>8</v>
       </c>
     </row>
@@ -5274,7 +5275,7 @@
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="2">
         <v>7</v>
       </c>
     </row>
@@ -5296,7 +5297,7 @@
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="2">
         <v>3</v>
       </c>
     </row>
@@ -5318,7 +5319,7 @@
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="2">
         <v>2</v>
       </c>
     </row>
@@ -5340,7 +5341,7 @@
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="2">
         <v>4</v>
       </c>
     </row>
@@ -5362,7 +5363,7 @@
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="2">
         <v>4</v>
       </c>
     </row>
@@ -5384,7 +5385,7 @@
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="2">
         <v>2</v>
       </c>
     </row>
@@ -5406,7 +5407,7 @@
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="2">
         <v>1</v>
       </c>
     </row>
@@ -5428,8 +5429,8 @@
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="F26">
-        <v>8</v>
+      <c r="F26" s="2">
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -5450,7 +5451,7 @@
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="2">
         <v>6</v>
       </c>
     </row>
@@ -5472,7 +5473,7 @@
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="2">
         <v>11</v>
       </c>
     </row>
@@ -5494,8 +5495,8 @@
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="F29">
-        <v>11</v>
+      <c r="F29" s="2">
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -5516,7 +5517,7 @@
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="2">
         <v>3</v>
       </c>
     </row>
@@ -5538,7 +5539,7 @@
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="2">
         <v>5</v>
       </c>
     </row>
@@ -5560,7 +5561,7 @@
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="2">
         <v>4</v>
       </c>
     </row>
@@ -5582,7 +5583,7 @@
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="2">
         <v>9</v>
       </c>
     </row>
@@ -5604,7 +5605,7 @@
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="F34">
+      <c r="F34" s="2">
         <v>4</v>
       </c>
     </row>
@@ -5626,7 +5627,7 @@
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
-      <c r="F35">
+      <c r="F35" s="2">
         <v>5</v>
       </c>
     </row>
@@ -5648,7 +5649,7 @@
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="F36">
+      <c r="F36" s="2">
         <v>6</v>
       </c>
     </row>
@@ -5670,8 +5671,8 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="F37">
-        <v>10</v>
+      <c r="F37" s="2">
+        <v>8</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -5692,7 +5693,7 @@
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
-      <c r="F38">
+      <c r="F38" s="2">
         <v>5</v>
       </c>
     </row>
@@ -5714,7 +5715,7 @@
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="F39">
+      <c r="F39" s="2">
         <v>6</v>
       </c>
     </row>
@@ -5736,7 +5737,7 @@
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
-      <c r="F40">
+      <c r="F40" s="2">
         <v>3</v>
       </c>
     </row>
@@ -5758,7 +5759,7 @@
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="F41">
+      <c r="F41" s="2">
         <v>3</v>
       </c>
     </row>
@@ -5780,8 +5781,8 @@
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="F42">
-        <v>7</v>
+      <c r="F42" s="2">
+        <v>6</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -5802,7 +5803,7 @@
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
-      <c r="F43">
+      <c r="F43" s="2">
         <v>1</v>
       </c>
     </row>
@@ -5824,7 +5825,7 @@
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
-      <c r="F44">
+      <c r="F44" s="2">
         <v>3</v>
       </c>
     </row>
@@ -5846,7 +5847,7 @@
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
-      <c r="F45">
+      <c r="F45" s="2">
         <v>3</v>
       </c>
     </row>
@@ -5868,7 +5869,7 @@
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
-      <c r="F46">
+      <c r="F46" s="2">
         <v>3</v>
       </c>
     </row>
@@ -5890,7 +5891,7 @@
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
-      <c r="F47">
+      <c r="F47" s="2">
         <v>4</v>
       </c>
     </row>
@@ -5912,7 +5913,7 @@
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
-      <c r="F48">
+      <c r="F48" s="2">
         <v>6</v>
       </c>
     </row>
@@ -5934,7 +5935,7 @@
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="F49">
+      <c r="F49" s="2">
         <v>2</v>
       </c>
     </row>
@@ -5956,7 +5957,7 @@
         <f t="shared" si="1"/>
         <v>49</v>
       </c>
-      <c r="F50">
+      <c r="F50" s="2">
         <v>4</v>
       </c>
     </row>
@@ -5978,7 +5979,7 @@
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="F51">
+      <c r="F51" s="2">
         <v>3</v>
       </c>
     </row>
@@ -6000,7 +6001,7 @@
         <f t="shared" si="1"/>
         <v>51</v>
       </c>
-      <c r="F52">
+      <c r="F52" s="2">
         <v>10</v>
       </c>
     </row>
@@ -6022,7 +6023,7 @@
         <f t="shared" si="1"/>
         <v>52</v>
       </c>
-      <c r="F53">
+      <c r="F53" s="2">
         <v>3</v>
       </c>
     </row>
@@ -6044,8 +6045,8 @@
         <f t="shared" si="1"/>
         <v>53</v>
       </c>
-      <c r="F54">
-        <v>6</v>
+      <c r="F54" s="2">
+        <v>5</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -6066,7 +6067,7 @@
         <f t="shared" si="1"/>
         <v>54</v>
       </c>
-      <c r="F55">
+      <c r="F55" s="2">
         <v>6</v>
       </c>
     </row>
@@ -6088,7 +6089,7 @@
         <f t="shared" si="1"/>
         <v>55</v>
       </c>
-      <c r="F56">
+      <c r="F56" s="2">
         <v>3</v>
       </c>
     </row>
@@ -6110,7 +6111,7 @@
         <f t="shared" si="1"/>
         <v>56</v>
       </c>
-      <c r="F57">
+      <c r="F57" s="2">
         <v>2</v>
       </c>
     </row>
@@ -6132,7 +6133,7 @@
         <f t="shared" si="1"/>
         <v>57</v>
       </c>
-      <c r="F58">
+      <c r="F58" s="2">
         <v>9</v>
       </c>
     </row>
@@ -6154,7 +6155,7 @@
         <f t="shared" si="1"/>
         <v>58</v>
       </c>
-      <c r="F59">
+      <c r="F59" s="2">
         <v>7</v>
       </c>
     </row>
@@ -6176,8 +6177,8 @@
         <f t="shared" si="1"/>
         <v>59</v>
       </c>
-      <c r="F60">
-        <v>8</v>
+      <c r="F60" s="2">
+        <v>7</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -6198,7 +6199,7 @@
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="F61">
+      <c r="F61" s="2">
         <v>10</v>
       </c>
     </row>
@@ -6220,8 +6221,8 @@
         <f t="shared" si="1"/>
         <v>61</v>
       </c>
-      <c r="F62">
-        <v>9</v>
+      <c r="F62" s="2">
+        <v>8</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -6242,7 +6243,7 @@
         <f t="shared" si="1"/>
         <v>62</v>
       </c>
-      <c r="F63">
+      <c r="F63" s="2">
         <v>5</v>
       </c>
     </row>
@@ -6264,7 +6265,7 @@
         <f t="shared" si="1"/>
         <v>63</v>
       </c>
-      <c r="F64">
+      <c r="F64" s="2">
         <v>5</v>
       </c>
     </row>
@@ -6286,8 +6287,8 @@
         <f t="shared" si="1"/>
         <v>64</v>
       </c>
-      <c r="F65">
-        <v>8</v>
+      <c r="F65" s="2">
+        <v>7</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -6308,7 +6309,7 @@
         <f t="shared" si="1"/>
         <v>65</v>
       </c>
-      <c r="F66">
+      <c r="F66" s="2">
         <v>5</v>
       </c>
     </row>
@@ -6330,7 +6331,7 @@
         <f t="shared" ref="E67:E130" si="3">(B67-2012)*52+C67-25</f>
         <v>66</v>
       </c>
-      <c r="F67">
+      <c r="F67" s="2">
         <v>8</v>
       </c>
     </row>
@@ -6352,7 +6353,7 @@
         <f t="shared" si="3"/>
         <v>67</v>
       </c>
-      <c r="F68">
+      <c r="F68" s="2">
         <v>5</v>
       </c>
     </row>
@@ -6374,7 +6375,7 @@
         <f t="shared" si="3"/>
         <v>68</v>
       </c>
-      <c r="F69">
+      <c r="F69" s="2">
         <v>6</v>
       </c>
     </row>
@@ -6396,7 +6397,7 @@
         <f t="shared" si="3"/>
         <v>69</v>
       </c>
-      <c r="F70">
+      <c r="F70" s="2">
         <v>4</v>
       </c>
     </row>
@@ -6418,7 +6419,7 @@
         <f t="shared" si="3"/>
         <v>70</v>
       </c>
-      <c r="F71">
+      <c r="F71" s="2">
         <v>4</v>
       </c>
     </row>
@@ -6440,7 +6441,7 @@
         <f t="shared" si="3"/>
         <v>71</v>
       </c>
-      <c r="F72">
+      <c r="F72" s="2">
         <v>6</v>
       </c>
     </row>
@@ -6462,8 +6463,8 @@
         <f t="shared" si="3"/>
         <v>72</v>
       </c>
-      <c r="F73">
-        <v>8</v>
+      <c r="F73" s="2">
+        <v>7</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
@@ -6484,8 +6485,8 @@
         <f t="shared" si="3"/>
         <v>73</v>
       </c>
-      <c r="F74">
-        <v>8</v>
+      <c r="F74" s="2">
+        <v>7</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -6506,7 +6507,7 @@
         <f t="shared" si="3"/>
         <v>74</v>
       </c>
-      <c r="F75">
+      <c r="F75" s="2">
         <v>6</v>
       </c>
     </row>
@@ -6528,8 +6529,8 @@
         <f t="shared" si="3"/>
         <v>75</v>
       </c>
-      <c r="F76">
-        <v>12</v>
+      <c r="F76" s="2">
+        <v>11</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
@@ -6550,7 +6551,7 @@
         <f t="shared" si="3"/>
         <v>76</v>
       </c>
-      <c r="F77">
+      <c r="F77" s="2">
         <v>5</v>
       </c>
     </row>
@@ -6572,7 +6573,7 @@
         <f t="shared" si="3"/>
         <v>77</v>
       </c>
-      <c r="F78">
+      <c r="F78" s="2">
         <v>6</v>
       </c>
     </row>
@@ -6594,8 +6595,8 @@
         <f t="shared" si="3"/>
         <v>78</v>
       </c>
-      <c r="F79">
-        <v>8</v>
+      <c r="F79" s="2">
+        <v>7</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -6616,7 +6617,7 @@
         <f t="shared" si="3"/>
         <v>79</v>
       </c>
-      <c r="F80">
+      <c r="F80" s="2">
         <v>5</v>
       </c>
     </row>
@@ -6638,7 +6639,7 @@
         <f t="shared" si="3"/>
         <v>80</v>
       </c>
-      <c r="F81">
+      <c r="F81" s="2">
         <v>8</v>
       </c>
     </row>
@@ -6660,7 +6661,7 @@
         <f t="shared" si="3"/>
         <v>81</v>
       </c>
-      <c r="F82">
+      <c r="F82" s="2">
         <v>7</v>
       </c>
     </row>
@@ -6682,7 +6683,7 @@
         <f t="shared" si="3"/>
         <v>82</v>
       </c>
-      <c r="F83">
+      <c r="F83" s="2">
         <v>5</v>
       </c>
     </row>
@@ -6704,7 +6705,7 @@
         <f t="shared" si="3"/>
         <v>83</v>
       </c>
-      <c r="F84">
+      <c r="F84" s="2">
         <v>3</v>
       </c>
     </row>
@@ -6726,7 +6727,7 @@
         <f t="shared" si="3"/>
         <v>84</v>
       </c>
-      <c r="F85">
+      <c r="F85" s="2">
         <v>3</v>
       </c>
     </row>
@@ -6748,7 +6749,7 @@
         <f t="shared" si="3"/>
         <v>85</v>
       </c>
-      <c r="F86">
+      <c r="F86" s="2">
         <v>4</v>
       </c>
     </row>
@@ -6770,7 +6771,7 @@
         <f t="shared" si="3"/>
         <v>86</v>
       </c>
-      <c r="F87">
+      <c r="F87" s="2">
         <v>3</v>
       </c>
     </row>
@@ -6792,8 +6793,8 @@
         <f t="shared" si="3"/>
         <v>87</v>
       </c>
-      <c r="F88">
-        <v>5</v>
+      <c r="F88" s="2">
+        <v>4</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -6814,7 +6815,7 @@
         <f t="shared" si="3"/>
         <v>88</v>
       </c>
-      <c r="F89">
+      <c r="F89" s="2">
         <v>1</v>
       </c>
     </row>
@@ -6836,7 +6837,7 @@
         <f t="shared" si="3"/>
         <v>89</v>
       </c>
-      <c r="F90">
+      <c r="F90" s="2">
         <v>5</v>
       </c>
     </row>
@@ -6858,7 +6859,7 @@
         <f t="shared" si="3"/>
         <v>90</v>
       </c>
-      <c r="F91">
+      <c r="F91" s="2">
         <v>2</v>
       </c>
     </row>
@@ -6880,7 +6881,7 @@
         <f t="shared" si="3"/>
         <v>91</v>
       </c>
-      <c r="F92">
+      <c r="F92" s="2">
         <v>5</v>
       </c>
     </row>
@@ -6902,7 +6903,7 @@
         <f t="shared" si="3"/>
         <v>92</v>
       </c>
-      <c r="F93">
+      <c r="F93" s="2">
         <v>5</v>
       </c>
     </row>
@@ -6924,8 +6925,8 @@
         <f t="shared" si="3"/>
         <v>93</v>
       </c>
-      <c r="F94">
-        <v>9</v>
+      <c r="F94" s="2">
+        <v>6</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
@@ -6946,7 +6947,7 @@
         <f t="shared" si="3"/>
         <v>94</v>
       </c>
-      <c r="F95">
+      <c r="F95" s="2">
         <v>3</v>
       </c>
     </row>
@@ -6968,7 +6969,7 @@
         <f t="shared" si="3"/>
         <v>95</v>
       </c>
-      <c r="F96">
+      <c r="F96" s="2">
         <v>3</v>
       </c>
     </row>
@@ -6990,7 +6991,7 @@
         <f t="shared" si="3"/>
         <v>96</v>
       </c>
-      <c r="F97">
+      <c r="F97" s="2">
         <v>4</v>
       </c>
     </row>
@@ -7012,7 +7013,7 @@
         <f t="shared" si="3"/>
         <v>97</v>
       </c>
-      <c r="F98">
+      <c r="F98" s="2">
         <v>6</v>
       </c>
     </row>
@@ -7034,7 +7035,7 @@
         <f t="shared" si="3"/>
         <v>98</v>
       </c>
-      <c r="F99">
+      <c r="F99" s="2">
         <v>6</v>
       </c>
     </row>
@@ -7056,7 +7057,7 @@
         <f t="shared" si="3"/>
         <v>99</v>
       </c>
-      <c r="F100">
+      <c r="F100" s="2">
         <v>4</v>
       </c>
     </row>
@@ -7078,8 +7079,8 @@
         <f t="shared" si="3"/>
         <v>100</v>
       </c>
-      <c r="F101">
-        <v>10</v>
+      <c r="F101" s="2">
+        <v>9</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
@@ -7100,7 +7101,7 @@
         <f t="shared" si="3"/>
         <v>101</v>
       </c>
-      <c r="F102">
+      <c r="F102" s="2">
         <v>3</v>
       </c>
     </row>
@@ -7122,7 +7123,7 @@
         <f t="shared" si="3"/>
         <v>102</v>
       </c>
-      <c r="F103">
+      <c r="F103" s="2">
         <v>8</v>
       </c>
     </row>
@@ -7144,7 +7145,7 @@
         <f t="shared" si="3"/>
         <v>103</v>
       </c>
-      <c r="F104">
+      <c r="F104" s="2">
         <v>7</v>
       </c>
     </row>
@@ -7166,7 +7167,7 @@
         <f t="shared" si="3"/>
         <v>104</v>
       </c>
-      <c r="F105">
+      <c r="F105" s="2">
         <v>3</v>
       </c>
     </row>
@@ -7188,7 +7189,7 @@
         <f t="shared" si="3"/>
         <v>105</v>
       </c>
-      <c r="F106">
+      <c r="F106" s="2">
         <v>4</v>
       </c>
     </row>
@@ -7210,7 +7211,7 @@
         <f t="shared" si="3"/>
         <v>106</v>
       </c>
-      <c r="F107">
+      <c r="F107" s="2">
         <v>7</v>
       </c>
     </row>
@@ -7232,7 +7233,7 @@
         <f t="shared" si="3"/>
         <v>107</v>
       </c>
-      <c r="F108">
+      <c r="F108" s="2">
         <v>4</v>
       </c>
     </row>
@@ -7254,7 +7255,7 @@
         <f t="shared" si="3"/>
         <v>108</v>
       </c>
-      <c r="F109">
+      <c r="F109" s="2">
         <v>7</v>
       </c>
     </row>
@@ -7276,7 +7277,7 @@
         <f t="shared" si="3"/>
         <v>109</v>
       </c>
-      <c r="F110">
+      <c r="F110" s="2">
         <v>8</v>
       </c>
     </row>
@@ -7298,8 +7299,8 @@
         <f t="shared" si="3"/>
         <v>110</v>
       </c>
-      <c r="F111">
-        <v>8</v>
+      <c r="F111" s="2">
+        <v>7</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
@@ -7320,7 +7321,7 @@
         <f t="shared" si="3"/>
         <v>111</v>
       </c>
-      <c r="F112">
+      <c r="F112" s="2">
         <v>2</v>
       </c>
     </row>
@@ -7342,7 +7343,7 @@
         <f t="shared" si="3"/>
         <v>112</v>
       </c>
-      <c r="F113">
+      <c r="F113" s="2">
         <v>4</v>
       </c>
     </row>
@@ -7364,7 +7365,7 @@
         <f t="shared" si="3"/>
         <v>113</v>
       </c>
-      <c r="F114">
+      <c r="F114" s="2">
         <v>3</v>
       </c>
     </row>
@@ -7386,7 +7387,7 @@
         <f t="shared" si="3"/>
         <v>114</v>
       </c>
-      <c r="F115">
+      <c r="F115" s="2">
         <v>8</v>
       </c>
     </row>
@@ -7408,7 +7409,7 @@
         <f t="shared" si="3"/>
         <v>115</v>
       </c>
-      <c r="F116">
+      <c r="F116" s="2">
         <v>8</v>
       </c>
     </row>
@@ -7430,8 +7431,8 @@
         <f t="shared" si="3"/>
         <v>116</v>
       </c>
-      <c r="F117">
-        <v>5</v>
+      <c r="F117" s="2">
+        <v>4</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
@@ -7452,8 +7453,8 @@
         <f t="shared" si="3"/>
         <v>117</v>
       </c>
-      <c r="F118">
-        <v>6</v>
+      <c r="F118" s="2">
+        <v>5</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
@@ -7474,7 +7475,7 @@
         <f t="shared" si="3"/>
         <v>118</v>
       </c>
-      <c r="F119">
+      <c r="F119" s="2">
         <v>8</v>
       </c>
     </row>
@@ -7496,7 +7497,7 @@
         <f t="shared" si="3"/>
         <v>119</v>
       </c>
-      <c r="F120">
+      <c r="F120" s="2">
         <v>3</v>
       </c>
     </row>
@@ -7518,7 +7519,7 @@
         <f t="shared" si="3"/>
         <v>120</v>
       </c>
-      <c r="F121">
+      <c r="F121" s="2">
         <v>5</v>
       </c>
     </row>
@@ -7540,8 +7541,8 @@
         <f t="shared" si="3"/>
         <v>121</v>
       </c>
-      <c r="F122">
-        <v>4</v>
+      <c r="F122" s="2">
+        <v>3</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
@@ -7562,7 +7563,7 @@
         <f t="shared" si="3"/>
         <v>122</v>
       </c>
-      <c r="F123">
+      <c r="F123" s="2">
         <v>5</v>
       </c>
     </row>
@@ -7584,7 +7585,7 @@
         <f t="shared" si="3"/>
         <v>123</v>
       </c>
-      <c r="F124">
+      <c r="F124" s="2">
         <v>5</v>
       </c>
     </row>
@@ -7606,8 +7607,8 @@
         <f t="shared" si="3"/>
         <v>124</v>
       </c>
-      <c r="F125">
-        <v>10</v>
+      <c r="F125" s="2">
+        <v>9</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
@@ -7628,7 +7629,7 @@
         <f t="shared" si="3"/>
         <v>125</v>
       </c>
-      <c r="F126">
+      <c r="F126" s="2">
         <v>5</v>
       </c>
     </row>
@@ -7650,7 +7651,7 @@
         <f t="shared" si="3"/>
         <v>126</v>
       </c>
-      <c r="F127">
+      <c r="F127" s="2">
         <v>4</v>
       </c>
     </row>
@@ -7672,7 +7673,7 @@
         <f t="shared" si="3"/>
         <v>127</v>
       </c>
-      <c r="F128">
+      <c r="F128" s="2">
         <v>6</v>
       </c>
     </row>
@@ -7694,7 +7695,7 @@
         <f t="shared" si="3"/>
         <v>128</v>
       </c>
-      <c r="F129">
+      <c r="F129" s="2">
         <v>4</v>
       </c>
     </row>
@@ -7716,7 +7717,7 @@
         <f t="shared" si="3"/>
         <v>129</v>
       </c>
-      <c r="F130">
+      <c r="F130" s="2">
         <v>3</v>
       </c>
     </row>
@@ -7738,7 +7739,7 @@
         <f t="shared" ref="E131:E194" si="5">(B131-2012)*52+C131-25</f>
         <v>130</v>
       </c>
-      <c r="F131">
+      <c r="F131" s="2">
         <v>2</v>
       </c>
     </row>
@@ -7760,7 +7761,7 @@
         <f t="shared" si="5"/>
         <v>131</v>
       </c>
-      <c r="F132">
+      <c r="F132" s="2">
         <v>2</v>
       </c>
     </row>
@@ -7782,7 +7783,7 @@
         <f t="shared" si="5"/>
         <v>132</v>
       </c>
-      <c r="F133">
+      <c r="F133" s="2">
         <v>3</v>
       </c>
     </row>
@@ -7804,7 +7805,7 @@
         <f t="shared" si="5"/>
         <v>133</v>
       </c>
-      <c r="F134">
+      <c r="F134" s="2">
         <v>4</v>
       </c>
     </row>
@@ -7826,7 +7827,7 @@
         <f t="shared" si="5"/>
         <v>134</v>
       </c>
-      <c r="F135">
+      <c r="F135" s="2">
         <v>4</v>
       </c>
     </row>
@@ -7848,7 +7849,7 @@
         <f t="shared" si="5"/>
         <v>135</v>
       </c>
-      <c r="F136">
+      <c r="F136" s="2">
         <v>3</v>
       </c>
     </row>
@@ -7870,7 +7871,7 @@
         <f t="shared" si="5"/>
         <v>136</v>
       </c>
-      <c r="F137">
+      <c r="F137" s="2">
         <v>2</v>
       </c>
     </row>
@@ -7892,7 +7893,7 @@
         <f t="shared" si="5"/>
         <v>137</v>
       </c>
-      <c r="F138">
+      <c r="F138" s="2">
         <v>2</v>
       </c>
     </row>
@@ -7914,7 +7915,7 @@
         <f t="shared" si="5"/>
         <v>138</v>
       </c>
-      <c r="F139">
+      <c r="F139" s="2">
         <v>3</v>
       </c>
     </row>
@@ -7936,7 +7937,7 @@
         <f t="shared" si="5"/>
         <v>139</v>
       </c>
-      <c r="F140">
+      <c r="F140" s="2">
         <v>7</v>
       </c>
     </row>
@@ -7958,7 +7959,7 @@
         <f t="shared" si="5"/>
         <v>140</v>
       </c>
-      <c r="F141">
+      <c r="F141" s="2">
         <v>5</v>
       </c>
     </row>
@@ -7980,7 +7981,7 @@
         <f t="shared" si="5"/>
         <v>141</v>
       </c>
-      <c r="F142">
+      <c r="F142" s="2">
         <v>2</v>
       </c>
     </row>
@@ -8002,7 +8003,7 @@
         <f t="shared" si="5"/>
         <v>142</v>
       </c>
-      <c r="F143">
+      <c r="F143" s="2">
         <v>1</v>
       </c>
     </row>
@@ -8024,8 +8025,8 @@
         <f t="shared" si="5"/>
         <v>143</v>
       </c>
-      <c r="F144">
-        <v>7</v>
+      <c r="F144" s="2">
+        <v>5</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
@@ -8046,7 +8047,7 @@
         <f t="shared" si="5"/>
         <v>144</v>
       </c>
-      <c r="F145">
+      <c r="F145" s="2">
         <v>2</v>
       </c>
     </row>
@@ -8068,8 +8069,8 @@
         <f t="shared" si="5"/>
         <v>145</v>
       </c>
-      <c r="F146">
-        <v>8</v>
+      <c r="F146" s="2">
+        <v>7</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
@@ -8090,7 +8091,7 @@
         <f t="shared" si="5"/>
         <v>146</v>
       </c>
-      <c r="F147">
+      <c r="F147" s="2">
         <v>2</v>
       </c>
     </row>
@@ -8112,7 +8113,7 @@
         <f t="shared" si="5"/>
         <v>147</v>
       </c>
-      <c r="F148">
+      <c r="F148" s="2">
         <v>3</v>
       </c>
     </row>
@@ -8134,7 +8135,7 @@
         <f t="shared" si="5"/>
         <v>148</v>
       </c>
-      <c r="F149">
+      <c r="F149" s="2">
         <v>5</v>
       </c>
     </row>
@@ -8156,8 +8157,8 @@
         <f t="shared" si="5"/>
         <v>149</v>
       </c>
-      <c r="F150">
-        <v>5</v>
+      <c r="F150" s="2">
+        <v>4</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
@@ -8178,7 +8179,7 @@
         <f t="shared" si="5"/>
         <v>150</v>
       </c>
-      <c r="F151">
+      <c r="F151" s="2">
         <v>6</v>
       </c>
     </row>
@@ -8200,7 +8201,7 @@
         <f t="shared" si="5"/>
         <v>151</v>
       </c>
-      <c r="F152">
+      <c r="F152" s="2">
         <v>7</v>
       </c>
     </row>
@@ -8222,7 +8223,7 @@
         <f t="shared" si="5"/>
         <v>152</v>
       </c>
-      <c r="F153">
+      <c r="F153" s="2">
         <v>5</v>
       </c>
     </row>
@@ -8244,7 +8245,7 @@
         <f t="shared" si="5"/>
         <v>153</v>
       </c>
-      <c r="F154">
+      <c r="F154" s="2">
         <v>9</v>
       </c>
     </row>
@@ -8266,7 +8267,7 @@
         <f t="shared" si="5"/>
         <v>154</v>
       </c>
-      <c r="F155">
+      <c r="F155" s="2">
         <v>5</v>
       </c>
     </row>
@@ -8288,7 +8289,7 @@
         <f t="shared" si="5"/>
         <v>155</v>
       </c>
-      <c r="F156">
+      <c r="F156" s="2">
         <v>3</v>
       </c>
     </row>
@@ -8310,7 +8311,7 @@
         <f t="shared" si="5"/>
         <v>156</v>
       </c>
-      <c r="F157">
+      <c r="F157" s="2">
         <v>3</v>
       </c>
     </row>
@@ -8332,7 +8333,7 @@
         <f t="shared" si="5"/>
         <v>157</v>
       </c>
-      <c r="F158">
+      <c r="F158" s="2">
         <v>7</v>
       </c>
     </row>
@@ -8354,8 +8355,8 @@
         <f t="shared" si="5"/>
         <v>158</v>
       </c>
-      <c r="F159">
-        <v>8</v>
+      <c r="F159" s="2">
+        <v>6</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
@@ -8376,7 +8377,7 @@
         <f t="shared" si="5"/>
         <v>159</v>
       </c>
-      <c r="F160">
+      <c r="F160" s="2">
         <v>5</v>
       </c>
     </row>
@@ -8398,7 +8399,7 @@
         <f t="shared" si="5"/>
         <v>160</v>
       </c>
-      <c r="F161">
+      <c r="F161" s="2">
         <v>4</v>
       </c>
     </row>
@@ -8420,7 +8421,7 @@
         <f t="shared" si="5"/>
         <v>161</v>
       </c>
-      <c r="F162">
+      <c r="F162" s="2">
         <v>3</v>
       </c>
     </row>
@@ -8442,7 +8443,7 @@
         <f t="shared" si="5"/>
         <v>162</v>
       </c>
-      <c r="F163">
+      <c r="F163" s="2">
         <v>4</v>
       </c>
     </row>
@@ -8464,7 +8465,7 @@
         <f t="shared" si="5"/>
         <v>163</v>
       </c>
-      <c r="F164">
+      <c r="F164" s="2">
         <v>6</v>
       </c>
     </row>
@@ -8486,7 +8487,7 @@
         <f t="shared" si="5"/>
         <v>164</v>
       </c>
-      <c r="F165">
+      <c r="F165" s="2">
         <v>3</v>
       </c>
     </row>
@@ -8508,7 +8509,7 @@
         <f t="shared" si="5"/>
         <v>165</v>
       </c>
-      <c r="F166">
+      <c r="F166" s="2">
         <v>6</v>
       </c>
     </row>
@@ -8530,7 +8531,7 @@
         <f t="shared" si="5"/>
         <v>166</v>
       </c>
-      <c r="F167">
+      <c r="F167" s="2">
         <v>5</v>
       </c>
     </row>
@@ -8552,7 +8553,7 @@
         <f t="shared" si="5"/>
         <v>167</v>
       </c>
-      <c r="F168">
+      <c r="F168" s="2">
         <v>2</v>
       </c>
     </row>
@@ -8574,7 +8575,7 @@
         <f t="shared" si="5"/>
         <v>168</v>
       </c>
-      <c r="F169">
+      <c r="F169" s="2">
         <v>5</v>
       </c>
     </row>
@@ -8596,7 +8597,7 @@
         <f t="shared" si="5"/>
         <v>169</v>
       </c>
-      <c r="F170">
+      <c r="F170" s="2">
         <v>3</v>
       </c>
     </row>
@@ -8618,7 +8619,7 @@
         <f t="shared" si="5"/>
         <v>170</v>
       </c>
-      <c r="F171">
+      <c r="F171" s="2">
         <v>4</v>
       </c>
     </row>
@@ -8640,7 +8641,7 @@
         <f t="shared" si="5"/>
         <v>171</v>
       </c>
-      <c r="F172">
+      <c r="F172" s="2">
         <v>2</v>
       </c>
     </row>
@@ -8662,8 +8663,8 @@
         <f t="shared" si="5"/>
         <v>172</v>
       </c>
-      <c r="F173">
-        <v>6</v>
+      <c r="F173" s="2">
+        <v>5</v>
       </c>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.25">
@@ -8684,7 +8685,7 @@
         <f t="shared" si="5"/>
         <v>173</v>
       </c>
-      <c r="F174">
+      <c r="F174" s="2">
         <v>9</v>
       </c>
     </row>
@@ -8706,7 +8707,7 @@
         <f t="shared" si="5"/>
         <v>174</v>
       </c>
-      <c r="F175">
+      <c r="F175" s="2">
         <v>6</v>
       </c>
     </row>
@@ -8728,7 +8729,7 @@
         <f t="shared" si="5"/>
         <v>175</v>
       </c>
-      <c r="F176">
+      <c r="F176" s="2">
         <v>4</v>
       </c>
     </row>
@@ -8750,7 +8751,7 @@
         <f t="shared" si="5"/>
         <v>176</v>
       </c>
-      <c r="F177">
+      <c r="F177" s="2">
         <v>7</v>
       </c>
     </row>
@@ -8772,7 +8773,7 @@
         <f t="shared" si="5"/>
         <v>177</v>
       </c>
-      <c r="F178">
+      <c r="F178" s="2">
         <v>5</v>
       </c>
     </row>
@@ -8794,7 +8795,7 @@
         <f t="shared" si="5"/>
         <v>178</v>
       </c>
-      <c r="F179">
+      <c r="F179" s="2">
         <v>4</v>
       </c>
     </row>
@@ -8816,8 +8817,8 @@
         <f t="shared" si="5"/>
         <v>179</v>
       </c>
-      <c r="F180">
-        <v>6</v>
+      <c r="F180" s="2">
+        <v>5</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.25">
@@ -8838,7 +8839,7 @@
         <f t="shared" si="5"/>
         <v>180</v>
       </c>
-      <c r="F181">
+      <c r="F181" s="2">
         <v>10</v>
       </c>
     </row>
@@ -8860,7 +8861,7 @@
         <f t="shared" si="5"/>
         <v>181</v>
       </c>
-      <c r="F182">
+      <c r="F182" s="2">
         <v>4</v>
       </c>
     </row>
@@ -8882,7 +8883,7 @@
         <f t="shared" si="5"/>
         <v>182</v>
       </c>
-      <c r="F183">
+      <c r="F183" s="2">
         <v>6</v>
       </c>
     </row>
@@ -8904,7 +8905,7 @@
         <f t="shared" si="5"/>
         <v>183</v>
       </c>
-      <c r="F184">
+      <c r="F184" s="2">
         <v>3</v>
       </c>
     </row>
@@ -8926,7 +8927,7 @@
         <f t="shared" si="5"/>
         <v>184</v>
       </c>
-      <c r="F185">
+      <c r="F185" s="2">
         <v>5</v>
       </c>
     </row>
@@ -8948,7 +8949,7 @@
         <f t="shared" si="5"/>
         <v>185</v>
       </c>
-      <c r="F186">
+      <c r="F186" s="2">
         <v>6</v>
       </c>
     </row>
@@ -8970,7 +8971,7 @@
         <f t="shared" si="5"/>
         <v>186</v>
       </c>
-      <c r="F187">
+      <c r="F187" s="2">
         <v>4</v>
       </c>
     </row>
@@ -8992,7 +8993,7 @@
         <f t="shared" si="5"/>
         <v>187</v>
       </c>
-      <c r="F188">
+      <c r="F188" s="2">
         <v>2</v>
       </c>
     </row>
@@ -9014,7 +9015,7 @@
         <f t="shared" si="5"/>
         <v>188</v>
       </c>
-      <c r="F189">
+      <c r="F189" s="2">
         <v>3</v>
       </c>
     </row>
@@ -9036,7 +9037,7 @@
         <f t="shared" si="5"/>
         <v>189</v>
       </c>
-      <c r="F190">
+      <c r="F190" s="2">
         <v>5</v>
       </c>
     </row>
@@ -9058,8 +9059,8 @@
         <f t="shared" si="5"/>
         <v>190</v>
       </c>
-      <c r="F191">
-        <v>4</v>
+      <c r="F191" s="2">
+        <v>3</v>
       </c>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.25">
@@ -9080,7 +9081,7 @@
         <f t="shared" si="5"/>
         <v>191</v>
       </c>
-      <c r="F192">
+      <c r="F192" s="2">
         <v>6</v>
       </c>
     </row>
@@ -9102,7 +9103,7 @@
         <f t="shared" si="5"/>
         <v>192</v>
       </c>
-      <c r="F193">
+      <c r="F193" s="2">
         <v>3</v>
       </c>
     </row>
@@ -9124,7 +9125,7 @@
         <f t="shared" si="5"/>
         <v>193</v>
       </c>
-      <c r="F194">
+      <c r="F194" s="2">
         <v>3</v>
       </c>
     </row>
@@ -9146,7 +9147,7 @@
         <f t="shared" ref="E195:E237" si="7">(B195-2012)*52+C195-25</f>
         <v>194</v>
       </c>
-      <c r="F195">
+      <c r="F195" s="2">
         <v>3</v>
       </c>
     </row>
@@ -9168,7 +9169,7 @@
         <f t="shared" si="7"/>
         <v>195</v>
       </c>
-      <c r="F196">
+      <c r="F196" s="2">
         <v>3</v>
       </c>
     </row>
@@ -9190,7 +9191,7 @@
         <f t="shared" si="7"/>
         <v>197</v>
       </c>
-      <c r="F197">
+      <c r="F197" s="2">
         <v>5</v>
       </c>
     </row>
@@ -9212,7 +9213,7 @@
         <f t="shared" si="7"/>
         <v>198</v>
       </c>
-      <c r="F198">
+      <c r="F198" s="2">
         <v>3</v>
       </c>
     </row>
@@ -9234,7 +9235,7 @@
         <f t="shared" si="7"/>
         <v>199</v>
       </c>
-      <c r="F199">
+      <c r="F199" s="2">
         <v>2</v>
       </c>
     </row>
@@ -9256,7 +9257,7 @@
         <f t="shared" si="7"/>
         <v>200</v>
       </c>
-      <c r="F200">
+      <c r="F200" s="2">
         <v>4</v>
       </c>
     </row>
@@ -9278,8 +9279,8 @@
         <f t="shared" si="7"/>
         <v>201</v>
       </c>
-      <c r="F201">
-        <v>6</v>
+      <c r="F201" s="2">
+        <v>4</v>
       </c>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.25">
@@ -9300,7 +9301,7 @@
         <f t="shared" si="7"/>
         <v>202</v>
       </c>
-      <c r="F202">
+      <c r="F202" s="2">
         <v>6</v>
       </c>
     </row>
@@ -9322,7 +9323,7 @@
         <f t="shared" si="7"/>
         <v>203</v>
       </c>
-      <c r="F203">
+      <c r="F203" s="2">
         <v>4</v>
       </c>
     </row>
@@ -9344,7 +9345,7 @@
         <f t="shared" si="7"/>
         <v>204</v>
       </c>
-      <c r="F204">
+      <c r="F204" s="2">
         <v>3</v>
       </c>
     </row>
@@ -9366,7 +9367,7 @@
         <f t="shared" si="7"/>
         <v>205</v>
       </c>
-      <c r="F205">
+      <c r="F205" s="2">
         <v>2</v>
       </c>
     </row>
@@ -9388,7 +9389,7 @@
         <f t="shared" si="7"/>
         <v>206</v>
       </c>
-      <c r="F206">
+      <c r="F206" s="2">
         <v>5</v>
       </c>
     </row>
@@ -9410,8 +9411,8 @@
         <f t="shared" si="7"/>
         <v>207</v>
       </c>
-      <c r="F207">
-        <v>13</v>
+      <c r="F207" s="2">
+        <v>10</v>
       </c>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.25">
@@ -9432,7 +9433,7 @@
         <f t="shared" si="7"/>
         <v>208</v>
       </c>
-      <c r="F208">
+      <c r="F208" s="2">
         <v>3</v>
       </c>
     </row>
@@ -9454,7 +9455,7 @@
         <f t="shared" si="7"/>
         <v>209</v>
       </c>
-      <c r="F209">
+      <c r="F209" s="2">
         <v>10</v>
       </c>
     </row>
@@ -9476,7 +9477,7 @@
         <f t="shared" si="7"/>
         <v>210</v>
       </c>
-      <c r="F210">
+      <c r="F210" s="2">
         <v>5</v>
       </c>
     </row>
@@ -9498,7 +9499,7 @@
         <f t="shared" si="7"/>
         <v>211</v>
       </c>
-      <c r="F211">
+      <c r="F211" s="2">
         <v>5</v>
       </c>
     </row>
@@ -9520,7 +9521,7 @@
         <f t="shared" si="7"/>
         <v>212</v>
       </c>
-      <c r="F212">
+      <c r="F212" s="2">
         <v>2</v>
       </c>
     </row>
@@ -9542,7 +9543,7 @@
         <f t="shared" si="7"/>
         <v>213</v>
       </c>
-      <c r="F213">
+      <c r="F213" s="2">
         <v>2</v>
       </c>
     </row>
@@ -9564,8 +9565,8 @@
         <f t="shared" si="7"/>
         <v>214</v>
       </c>
-      <c r="F214">
-        <v>5</v>
+      <c r="F214" s="2">
+        <v>4</v>
       </c>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.25">
@@ -9586,7 +9587,7 @@
         <f t="shared" si="7"/>
         <v>215</v>
       </c>
-      <c r="F215">
+      <c r="F215" s="2">
         <v>6</v>
       </c>
     </row>
@@ -9608,7 +9609,7 @@
         <f t="shared" si="7"/>
         <v>216</v>
       </c>
-      <c r="F216">
+      <c r="F216" s="2">
         <v>4</v>
       </c>
     </row>
@@ -9630,7 +9631,7 @@
         <f t="shared" si="7"/>
         <v>217</v>
       </c>
-      <c r="F217">
+      <c r="F217" s="2">
         <v>5</v>
       </c>
     </row>
@@ -9652,8 +9653,8 @@
         <f t="shared" si="7"/>
         <v>218</v>
       </c>
-      <c r="F218">
-        <v>10</v>
+      <c r="F218" s="2">
+        <v>8</v>
       </c>
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.25">
@@ -9674,7 +9675,7 @@
         <f t="shared" si="7"/>
         <v>219</v>
       </c>
-      <c r="F219">
+      <c r="F219" s="2">
         <v>3</v>
       </c>
     </row>
@@ -9696,7 +9697,7 @@
         <f t="shared" si="7"/>
         <v>220</v>
       </c>
-      <c r="F220">
+      <c r="F220" s="2">
         <v>3</v>
       </c>
     </row>
@@ -9718,7 +9719,7 @@
         <f t="shared" si="7"/>
         <v>221</v>
       </c>
-      <c r="F221">
+      <c r="F221" s="2">
         <v>3</v>
       </c>
     </row>
@@ -9740,7 +9741,7 @@
         <f t="shared" si="7"/>
         <v>222</v>
       </c>
-      <c r="F222">
+      <c r="F222" s="2">
         <v>6</v>
       </c>
     </row>
@@ -9762,7 +9763,7 @@
         <f t="shared" si="7"/>
         <v>223</v>
       </c>
-      <c r="F223">
+      <c r="F223" s="2">
         <v>5</v>
       </c>
     </row>
@@ -9784,7 +9785,7 @@
         <f t="shared" si="7"/>
         <v>224</v>
       </c>
-      <c r="F224">
+      <c r="F224" s="2">
         <v>7</v>
       </c>
     </row>
@@ -9806,7 +9807,7 @@
         <f t="shared" si="7"/>
         <v>225</v>
       </c>
-      <c r="F225">
+      <c r="F225" s="2">
         <v>5</v>
       </c>
     </row>
@@ -9828,7 +9829,7 @@
         <f t="shared" si="7"/>
         <v>226</v>
       </c>
-      <c r="F226">
+      <c r="F226" s="2">
         <v>3</v>
       </c>
     </row>
@@ -9850,7 +9851,7 @@
         <f t="shared" si="7"/>
         <v>227</v>
       </c>
-      <c r="F227">
+      <c r="F227" s="2">
         <v>4</v>
       </c>
     </row>
@@ -9872,7 +9873,7 @@
         <f t="shared" si="7"/>
         <v>228</v>
       </c>
-      <c r="F228">
+      <c r="F228" s="2">
         <v>5</v>
       </c>
     </row>
@@ -9894,7 +9895,7 @@
         <f t="shared" si="7"/>
         <v>229</v>
       </c>
-      <c r="F229">
+      <c r="F229" s="2">
         <v>6</v>
       </c>
     </row>
@@ -9916,7 +9917,7 @@
         <f t="shared" si="7"/>
         <v>230</v>
       </c>
-      <c r="F230">
+      <c r="F230" s="2">
         <v>1</v>
       </c>
     </row>
@@ -9938,7 +9939,7 @@
         <f t="shared" si="7"/>
         <v>231</v>
       </c>
-      <c r="F231">
+      <c r="F231" s="2">
         <v>3</v>
       </c>
     </row>
@@ -9960,7 +9961,7 @@
         <f t="shared" si="7"/>
         <v>232</v>
       </c>
-      <c r="F232">
+      <c r="F232" s="2">
         <v>5</v>
       </c>
     </row>
@@ -9982,7 +9983,7 @@
         <f t="shared" si="7"/>
         <v>233</v>
       </c>
-      <c r="F233">
+      <c r="F233" s="2">
         <v>4</v>
       </c>
     </row>
@@ -10004,7 +10005,7 @@
         <f t="shared" si="7"/>
         <v>234</v>
       </c>
-      <c r="F234">
+      <c r="F234" s="2">
         <v>2</v>
       </c>
     </row>
@@ -10026,8 +10027,8 @@
         <f t="shared" si="7"/>
         <v>235</v>
       </c>
-      <c r="F235">
-        <v>7</v>
+      <c r="F235" s="2">
+        <v>5</v>
       </c>
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.25">
@@ -10048,7 +10049,7 @@
         <f t="shared" si="7"/>
         <v>237</v>
       </c>
-      <c r="F236">
+      <c r="F236" s="2">
         <v>1</v>
       </c>
     </row>
@@ -10070,7 +10071,7 @@
         <f t="shared" si="7"/>
         <v>236</v>
       </c>
-      <c r="F237">
+      <c r="F237" s="2">
         <v>4</v>
       </c>
     </row>

</xml_diff>